<commit_message>
[DOC] 요청 사항 update - 2/27 meeting
</commit_message>
<xml_diff>
--- a/Plasma LF Review Data V1.0.xlsx
+++ b/Plasma LF Review Data V1.0.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GEN MCU" sheetId="1" r:id="rId1"/>
     <sheet name="GEN" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Ctrl PCB" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -144,6 +144,34 @@
   </si>
   <si>
     <t>Load Short 발생시 2차측 전압이 역으로 유기되는지 확인 필요 - Pipette dead 원인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회로 보강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 부품을 SMT type 으로 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stepping motor Control 추가 - 2ea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검토 사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>압력 sensor 변경 검토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heater control 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불필요 block 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -184,7 +212,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -372,11 +400,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -448,12 +550,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -463,6 +559,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -523,7 +643,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,7 +678,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -769,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1068,7 +1188,7 @@
   <dimension ref="B1:E28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1095,202 +1215,202 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="25">
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="25">
+      <c r="B8" s="33">
         <v>2</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="25">
+      <c r="B12" s="33">
         <v>3</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="26"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27" t="s">
+      <c r="B13" s="33"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="28"/>
+      <c r="E13" s="26"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="30"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="30"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="30"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="30"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="30"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="30"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="30"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="30"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="30"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
     </row>
     <row r="28" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1309,12 +1429,212 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.875" customWidth="1"/>
+    <col min="3" max="3" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="34">
+        <v>1</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="26"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="34">
+        <v>2</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="34">
+        <v>3</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="28"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="28"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="28"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="28"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="28"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="28"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="28"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="28"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="28"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="28"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="28"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="28"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="26"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="28"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="28"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
+    </row>
+    <row r="28" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[DOC] Femto sheet 추가
</commit_message>
<xml_diff>
--- a/Plasma LF Review Data V1.0.xlsx
+++ b/Plasma LF Review Data V1.0.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="GEN MCU" sheetId="1" r:id="rId1"/>
-    <sheet name="GEN" sheetId="2" r:id="rId2"/>
-    <sheet name="Ctrl MCU" sheetId="4" r:id="rId3"/>
-    <sheet name="Ctrl PCB" sheetId="3" r:id="rId4"/>
+    <sheet name="Femto work" sheetId="5" r:id="rId1"/>
+    <sheet name="GEN MCU" sheetId="1" r:id="rId2"/>
+    <sheet name="GEN" sheetId="2" r:id="rId3"/>
+    <sheet name="Ctrl MCU" sheetId="4" r:id="rId4"/>
+    <sheet name="Ctrl PCB" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,6 +228,30 @@
   <si>
     <t>Current Sensing용 ADC0에  Zener diode(BZT52C5V1S) 추가
 OP_OUT용 G17에  Zener diode(BZT52C5V1S) 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Touch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Program UI image 전달</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -259,7 +284,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +294,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -629,48 +660,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -975,9 +1033,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="11.25" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="6" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="9" style="49"/>
+    <col min="8" max="8" width="48.125" customWidth="1"/>
+    <col min="9" max="9" width="33.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="53">
+        <v>1</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="55">
+        <v>43194</v>
+      </c>
+      <c r="F6" s="55"/>
+      <c r="G6" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="57"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="25">
+        <v>2</v>
+      </c>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="25">
+        <v>3</v>
+      </c>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="25">
+        <v>4</v>
+      </c>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="25">
+        <v>5</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="25">
+        <v>6</v>
+      </c>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="25">
+        <v>7</v>
+      </c>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="25">
+        <v>8</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="25">
+        <v>9</v>
+      </c>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="25">
+        <v>10</v>
+      </c>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="25">
+        <v>11</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="25">
+        <v>12</v>
+      </c>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="25">
+        <v>13</v>
+      </c>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="25">
+        <v>14</v>
+      </c>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="25">
+        <v>15</v>
+      </c>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="25">
+        <v>16</v>
+      </c>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="25">
+        <v>17</v>
+      </c>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="25">
+        <v>18</v>
+      </c>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="25">
+        <v>19</v>
+      </c>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="25">
+        <v>20</v>
+      </c>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="25">
+        <v>21</v>
+      </c>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="25">
+        <v>22</v>
+      </c>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="25">
+        <v>23</v>
+      </c>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="23"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="25">
+        <v>24</v>
+      </c>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
+    </row>
+    <row r="30" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="25">
+        <v>25</v>
+      </c>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="28"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -1010,121 +1431,121 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="44">
+      <c r="B5" s="42">
         <v>1</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="43">
         <v>43150</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="46" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="37">
+      <c r="B6" s="35">
         <v>2</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="36">
         <v>43150</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="39" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B7" s="37">
+      <c r="B7" s="35">
         <v>3</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="36">
         <v>43150</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="37">
+      <c r="B8" s="35">
         <v>4</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="36">
         <v>43150</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B9" s="37">
+      <c r="B9" s="35">
         <v>5</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="36">
         <v>43169</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="37">
+      <c r="B10" s="35">
         <v>6</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="36">
         <v>43193</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="41" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="37">
+      <c r="B11" s="35">
         <v>7</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="36">
         <v>43193</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="41" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1295,7 +1716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E28"/>
   <sheetViews>
@@ -1327,10 +1748,10 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="36">
+      <c r="B3" s="48">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="47" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="22" t="s">
@@ -1341,8 +1762,8 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="35"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="22" t="s">
         <v>8</v>
       </c>
@@ -1351,34 +1772,34 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="36"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="47"/>
       <c r="D5" s="22" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="23"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="36"/>
-      <c r="C6" s="35"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="23"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="36"/>
-      <c r="C7" s="35"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="22" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="36">
+      <c r="B8" s="48">
         <v>2</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="47" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="24" t="s">
@@ -1389,8 +1810,8 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="36"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="22" t="s">
         <v>14</v>
       </c>
@@ -1399,8 +1820,8 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="36"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="22" t="s">
         <v>16</v>
       </c>
@@ -1409,16 +1830,16 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="36"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="22"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="36">
+      <c r="B12" s="48">
         <v>3</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="47" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="22" t="s">
@@ -1427,8 +1848,8 @@
       <c r="E12" s="23"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="36"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="22" t="s">
         <v>33</v>
       </c>
@@ -1539,7 +1960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F26"/>
   <sheetViews>
@@ -1808,7 +2229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E28"/>
   <sheetViews>

</xml_diff>